<commit_message>
add sigma conu cvza
</commit_message>
<xml_diff>
--- a/control_carga.xlsx
+++ b/control_carga.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\srvdc\Unidad Personal\glorenzo\Documents\UiPath\carga_comprobantes_sigma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3FC823A-16F5-40FE-9AA4-88B40C2B8C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F065DCE-46F2-42D6-B336-6A71F5DCA400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -393,10 +393,10 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A2" sqref="A2:C57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="33.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="125.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>

</xml_diff>